<commit_message>
Added conda and pip environment dependency files and updated Readme.
</commit_message>
<xml_diff>
--- a/Dec2021ExperimentResults/BuzzwireSurveyData.xlsx
+++ b/Dec2021ExperimentResults/BuzzwireSurveyData.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr hidePivotFieldList="1"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au657021\Gitlab_AU\BuzzwireExperimentDataAnalysis\Dec2021ExperimentResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7056" windowHeight="4836" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7050" windowHeight="4830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="10" r:id="rId1"/>
@@ -24,6 +24,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId8"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3995" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3996" uniqueCount="77">
   <si>
     <t>Completion time</t>
   </si>
@@ -262,9 +263,6 @@
     <t>Diff_Efficacy</t>
   </si>
   <si>
-    <t>Count of Gender</t>
-  </si>
-  <si>
     <t>Count of Immersion8</t>
   </si>
   <si>
@@ -272,6 +270,9 @@
   </si>
   <si>
     <t>Eff2</t>
+  </si>
+  <si>
+    <t>Count of Prev_VR</t>
   </si>
 </sst>
 </file>
@@ -990,7 +991,12 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Prev_VR" numFmtId="0">
-      <sharedItems/>
+      <sharedItems count="4">
+        <s v="1-5"/>
+        <s v="5-10"/>
+        <s v="More than 10"/>
+        <s v="Never"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Presence1" numFmtId="0">
       <sharedItems/>
@@ -1114,7 +1120,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Neither Agree or Disagree"/>
@@ -1155,7 +1161,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Disagree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -1196,7 +1202,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -1237,7 +1243,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Neither Agree or Disagree"/>
@@ -1278,7 +1284,7 @@
     <n v="7"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="5-10"/>
+    <x v="1"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Neither Agree or Disagree"/>
@@ -1319,7 +1325,7 @@
     <n v="6"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -1360,7 +1366,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="2"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -1401,7 +1407,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -1442,7 +1448,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="5-10"/>
+    <x v="1"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -1483,7 +1489,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
     <s v="Agree"/>
@@ -1524,7 +1530,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="5-10"/>
+    <x v="1"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
     <s v="Agree"/>
@@ -1565,7 +1571,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -1606,7 +1612,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat Agree"/>
     <s v="Strongly Agree"/>
     <s v="Somewhat Agree"/>
@@ -1647,7 +1653,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
@@ -1688,7 +1694,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Strongly Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -1729,7 +1735,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -1770,7 +1776,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -1811,7 +1817,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Agree"/>
     <s v="Strongly Agree"/>
     <s v="Strongly Agree"/>
@@ -1852,7 +1858,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="5-10"/>
+    <x v="1"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
@@ -1893,7 +1899,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
@@ -1934,7 +1940,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -1975,7 +1981,7 @@
     <n v="4"/>
     <s v="35-44"/>
     <x v="1"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2016,7 +2022,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2057,7 +2063,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Disagree"/>
@@ -2098,7 +2104,7 @@
     <n v="6"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
@@ -2139,7 +2145,7 @@
     <n v="6"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Neither Agree or Disagree"/>
@@ -2180,7 +2186,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Disagree"/>
     <s v="Agree"/>
     <s v="Somewhat Agree"/>
@@ -2221,7 +2227,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2262,7 +2268,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2303,7 +2309,7 @@
     <n v="1"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Disagree"/>
     <s v="Strongly Disagree"/>
     <s v="Agree"/>
@@ -2344,7 +2350,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Strongly Agree"/>
     <s v="Strongly Agree"/>
@@ -2385,7 +2391,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
@@ -2426,7 +2432,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Strongly Agree"/>
@@ -2467,7 +2473,7 @@
     <n v="5"/>
     <s v="45-54"/>
     <x v="2"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -2508,7 +2514,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Disagree"/>
     <s v="Neither Agree or Disagree"/>
@@ -2549,7 +2555,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
     <s v="Strongly Agree"/>
@@ -2590,7 +2596,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2631,7 +2637,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat Agree"/>
     <s v="Strongly Agree"/>
     <s v="Strongly Agree"/>
@@ -2672,7 +2678,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat_x000a_  Disagree"/>
@@ -2713,7 +2719,7 @@
     <n v="2"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2754,7 +2760,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2795,7 +2801,7 @@
     <n v="4"/>
     <s v="Under 18"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -2836,7 +2842,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Disagree"/>
     <s v="Neither Agree or Disagree"/>
@@ -2877,7 +2883,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Agree"/>
     <s v="Somewhat Agree"/>
@@ -2918,7 +2924,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Disagree"/>
     <s v="Disagree"/>
     <s v="Disagree"/>
@@ -2959,7 +2965,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Disagree"/>
@@ -3000,7 +3006,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -3041,7 +3047,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Disagree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -3082,7 +3088,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Strongly Disagree"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Neither Agree or Disagree"/>
@@ -3123,7 +3129,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -3164,7 +3170,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="5-10"/>
+    <x v="1"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -3205,7 +3211,7 @@
     <n v="7"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="5-10"/>
+    <x v="1"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
     <s v="Strongly Agree"/>
@@ -3246,7 +3252,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -3287,7 +3293,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
@@ -3328,7 +3334,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
@@ -3369,7 +3375,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
@@ -3410,7 +3416,7 @@
     <n v="6"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
     <s v="Agree"/>
@@ -3451,7 +3457,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
@@ -3492,7 +3498,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="5-10"/>
+    <x v="1"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -3533,7 +3539,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
@@ -3574,7 +3580,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Disagree"/>
     <s v="Agree"/>
     <s v="Somewhat Agree"/>
@@ -3615,7 +3621,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -3656,7 +3662,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Strongly Agree"/>
@@ -3697,7 +3703,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
@@ -3738,7 +3744,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Strongly Agree"/>
@@ -3779,7 +3785,7 @@
     <n v="2"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Agree"/>
@@ -3820,7 +3826,7 @@
     <n v="2"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Neither Agree or Disagree"/>
@@ -3861,7 +3867,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -3902,7 +3908,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Somewhat Agree"/>
@@ -3943,7 +3949,7 @@
     <n v="5"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -3984,7 +3990,7 @@
     <n v="6"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -4025,7 +4031,7 @@
     <n v="5"/>
     <s v="35-44"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -4066,7 +4072,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Agree"/>
@@ -4107,7 +4113,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -4148,7 +4154,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
     <s v="Somewhat Agree"/>
@@ -4189,7 +4195,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Neither Agree or Disagree"/>
@@ -4230,7 +4236,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -4271,7 +4277,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
@@ -4312,7 +4318,7 @@
     <n v="3"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -4353,7 +4359,7 @@
     <n v="6"/>
     <s v="18-24"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Strongly Agree"/>
     <s v="Agree"/>
@@ -4394,7 +4400,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -4435,7 +4441,7 @@
     <n v="4"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Somewhat Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Agree"/>
@@ -4476,7 +4482,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Agree"/>
     <s v="Somewhat Agree"/>
     <s v="Strongly Agree"/>
@@ -4517,7 +4523,7 @@
     <n v="4"/>
     <s v="18-24"/>
     <x v="0"/>
-    <s v="Never"/>
+    <x v="3"/>
     <s v="Somewhat Agree"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Somewhat Agree"/>
@@ -4558,7 +4564,7 @@
     <n v="3"/>
     <s v="25-34"/>
     <x v="1"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Agree"/>
@@ -4599,7 +4605,7 @@
     <n v="3"/>
     <s v="45-54"/>
     <x v="1"/>
-    <s v="More than 10"/>
+    <x v="2"/>
     <s v="Neither Agree or Disagree"/>
     <s v="Agree"/>
     <s v="Agree"/>
@@ -4640,7 +4646,7 @@
     <n v="5"/>
     <s v="25-34"/>
     <x v="0"/>
-    <s v="1-5"/>
+    <x v="0"/>
     <s v="Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
     <s v="Somewhat_x000a_  Disagree"/>
@@ -4679,7 +4685,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable15" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A11:E15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <location ref="A11:F15" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="39">
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
@@ -4692,7 +4698,7 @@
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisCol" dataField="1" showAll="0">
+    <pivotField showAll="0">
       <items count="4">
         <item x="1"/>
         <item x="0"/>
@@ -4700,7 +4706,15 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
@@ -4749,9 +4763,9 @@
     </i>
   </rowItems>
   <colFields count="1">
-    <field x="5"/>
+    <field x="6"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="5">
     <i>
       <x/>
     </i>
@@ -4761,12 +4775,15 @@
     <i>
       <x v="2"/>
     </i>
+    <i>
+      <x v="3"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Count of Gender" fld="5" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Count of Prev_VR" fld="6" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -5389,27 +5406,27 @@
       <selection sqref="A1:AM43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" customWidth="1"/>
-    <col min="8" max="16" width="12.33203125" customWidth="1"/>
-    <col min="17" max="21" width="13.33203125" customWidth="1"/>
-    <col min="22" max="30" width="13.6640625" customWidth="1"/>
-    <col min="31" max="32" width="14.6640625" customWidth="1"/>
-    <col min="33" max="33" width="12.6640625" customWidth="1"/>
-    <col min="34" max="34" width="17.44140625" customWidth="1"/>
-    <col min="35" max="35" width="18.109375" customWidth="1"/>
-    <col min="36" max="36" width="19.44140625" customWidth="1"/>
-    <col min="37" max="37" width="14.5546875" customWidth="1"/>
-    <col min="39" max="39" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="21" width="13.28515625" customWidth="1"/>
+    <col min="22" max="30" width="13.7109375" customWidth="1"/>
+    <col min="31" max="32" width="14.7109375" customWidth="1"/>
+    <col min="33" max="33" width="12.7109375" customWidth="1"/>
+    <col min="34" max="34" width="17.42578125" customWidth="1"/>
+    <col min="35" max="35" width="18.140625" customWidth="1"/>
+    <col min="36" max="36" width="19.42578125" customWidth="1"/>
+    <col min="37" max="37" width="14.5703125" customWidth="1"/>
+    <col min="39" max="39" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5528,7 +5545,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>44538.660694444443</v>
       </c>
@@ -5647,7 +5664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>44529.407673611109</v>
       </c>
@@ -5766,7 +5783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>44529.441354166665</v>
       </c>
@@ -5885,7 +5902,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>44538.564131944448</v>
       </c>
@@ -6004,7 +6021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>44529.482835648145</v>
       </c>
@@ -6123,7 +6140,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>44538.496157407404</v>
       </c>
@@ -6242,7 +6259,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>44529.590300925927</v>
       </c>
@@ -6361,7 +6378,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>44538.406469907408</v>
       </c>
@@ -6480,7 +6497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>44529.619490740741</v>
       </c>
@@ -6599,7 +6616,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>44537.656435185185</v>
       </c>
@@ -6718,7 +6735,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>44529.701921296299</v>
       </c>
@@ -6837,7 +6854,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>44537.534548611111</v>
       </c>
@@ -6956,7 +6973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>44530.4059375</v>
       </c>
@@ -7075,7 +7092,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>44530.439421296294</v>
       </c>
@@ -7194,7 +7211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>44537.483495370368</v>
       </c>
@@ -7313,7 +7330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>44537.397696759261</v>
       </c>
@@ -7432,7 +7449,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>44530.489942129629</v>
       </c>
@@ -7551,7 +7568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>44536.697928240741</v>
       </c>
@@ -7670,7 +7687,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>44530.575729166667</v>
       </c>
@@ -7789,7 +7806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>44536.577118055553</v>
       </c>
@@ -7908,7 +7925,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>44530.614328703705</v>
       </c>
@@ -8027,7 +8044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>44536.530462962961</v>
       </c>
@@ -8146,7 +8163,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>44530.656886574077</v>
       </c>
@@ -8265,7 +8282,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>44536.481076388889</v>
       </c>
@@ -8384,7 +8401,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>44536.408541666664</v>
       </c>
@@ -8503,7 +8520,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>44534.617881944447</v>
       </c>
@@ -8622,7 +8639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>44531.417361111111</v>
       </c>
@@ -8741,7 +8758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>44534.539907407408</v>
       </c>
@@ -8860,7 +8877,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>44531.479768518519</v>
       </c>
@@ -8979,7 +8996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>44531.538587962961</v>
       </c>
@@ -9098,7 +9115,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="6">
         <v>44534.450266203705</v>
       </c>
@@ -9217,7 +9234,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>44534.400462962964</v>
       </c>
@@ -9336,7 +9353,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>44531.617743055554</v>
       </c>
@@ -9455,7 +9472,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>44531.656631944446</v>
       </c>
@@ -9574,7 +9591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>44533.663969907408</v>
       </c>
@@ -9693,7 +9710,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>44531.679027777776</v>
       </c>
@@ -9812,7 +9829,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>44533.56958333333</v>
       </c>
@@ -9931,7 +9948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>44533.537743055553</v>
       </c>
@@ -10050,7 +10067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>44532.657650462963</v>
       </c>
@@ -10169,7 +10186,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>44533.482638888891</v>
       </c>
@@ -10288,7 +10305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
         <v>44533.404999999999</v>
       </c>
@@ -10407,7 +10424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:39" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:39" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>44533.445590277777</v>
       </c>
@@ -10536,26 +10553,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E29"/>
+  <dimension ref="A3:F29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>35</v>
       </c>
@@ -10566,7 +10583,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
@@ -10577,7 +10594,7 @@
         <v>4.4761904761904763</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>33</v>
       </c>
@@ -10588,7 +10605,7 @@
         <v>4.2444444444444445</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
@@ -10599,89 +10616,103 @@
         <v>4.3563218390804597</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="3">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="D13" s="3">
         <v>2</v>
       </c>
       <c r="E13" s="3">
+        <v>5</v>
+      </c>
+      <c r="F13" s="3">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="3">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C14" s="3">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>6</v>
+      </c>
       <c r="E14" s="3">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3">
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="3">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C15" s="3">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E15" s="3">
+        <v>12</v>
+      </c>
+      <c r="F15" s="3">
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
@@ -10695,7 +10726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>14</v>
       </c>
@@ -10709,7 +10740,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>13</v>
       </c>
@@ -10723,7 +10754,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>11</v>
       </c>
@@ -10737,7 +10768,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>16</v>
       </c>
@@ -10751,7 +10782,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>10</v>
       </c>
@@ -10765,7 +10796,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
@@ -10779,7 +10810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
@@ -10791,7 +10822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>36</v>
       </c>
@@ -10814,18 +10845,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="39" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10947,7 +10978,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44529.403854166703</v>
       </c>
@@ -11070,7 +11101,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44529.407673611102</v>
       </c>
@@ -11193,7 +11224,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44529.441354166702</v>
       </c>
@@ -11316,7 +11347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44529.481226851902</v>
       </c>
@@ -11439,7 +11470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44529.482835648101</v>
       </c>
@@ -11562,7 +11593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44529.530092592599</v>
       </c>
@@ -11685,7 +11716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44529.590300925898</v>
       </c>
@@ -11808,7 +11839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44529.6078935185</v>
       </c>
@@ -11931,7 +11962,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44529.619490740697</v>
       </c>
@@ -12054,7 +12085,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>44529.660740740699</v>
       </c>
@@ -12177,7 +12208,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>44529.701921296299</v>
       </c>
@@ -12300,7 +12331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>44530.397777777798</v>
       </c>
@@ -12423,7 +12454,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>44530.4059375</v>
       </c>
@@ -12546,7 +12577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>44530.439421296302</v>
       </c>
@@ -12669,7 +12700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>44530.450405092597</v>
       </c>
@@ -12792,7 +12823,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>44530.485740740703</v>
       </c>
@@ -12915,7 +12946,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>44530.4899421296</v>
       </c>
@@ -13038,7 +13069,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>44530.533564814803</v>
       </c>
@@ -13161,7 +13192,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>44530.575729166703</v>
       </c>
@@ -13284,7 +13315,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>44530.578113425901</v>
       </c>
@@ -13407,7 +13438,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>44530.614328703698</v>
       </c>
@@ -13530,7 +13561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>44530.6170486111</v>
       </c>
@@ -13653,7 +13684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>44530.656886574099</v>
       </c>
@@ -13776,7 +13807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>44530.668263888903</v>
       </c>
@@ -13899,7 +13930,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>44530.699606481503</v>
       </c>
@@ -14022,7 +14053,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>44531.415416666699</v>
       </c>
@@ -14145,7 +14176,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>44531.417361111096</v>
       </c>
@@ -14268,7 +14299,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>44531.443043981497</v>
       </c>
@@ -14391,7 +14422,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>44531.479768518497</v>
       </c>
@@ -14514,7 +14545,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>44531.538587962998</v>
       </c>
@@ -14637,7 +14668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>44531.5761921296</v>
       </c>
@@ -14760,7 +14791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>44531.610416666699</v>
       </c>
@@ -14883,7 +14914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>44531.617743055598</v>
       </c>
@@ -15006,7 +15037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>44531.656631944403</v>
       </c>
@@ -15129,7 +15160,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>44531.657337962999</v>
       </c>
@@ -15252,7 +15283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>44531.679027777798</v>
       </c>
@@ -15375,7 +15406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>44532.543668981503</v>
       </c>
@@ -15498,7 +15529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>44532.613854166702</v>
       </c>
@@ -15621,7 +15652,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>44532.657650462999</v>
       </c>
@@ -15744,7 +15775,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>44532.702337962997</v>
       </c>
@@ -15867,7 +15898,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>44533.404999999999</v>
       </c>
@@ -15990,7 +16021,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>44533.440300925897</v>
       </c>
@@ -16113,7 +16144,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>44533.445590277799</v>
       </c>
@@ -16236,7 +16267,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44533.476909722202</v>
       </c>
@@ -16359,7 +16390,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44533.482638888898</v>
       </c>
@@ -16482,7 +16513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>44533.525902777801</v>
       </c>
@@ -16605,7 +16636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44533.537743055596</v>
       </c>
@@ -16728,7 +16759,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>44533.556898148097</v>
       </c>
@@ -16851,7 +16882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>44533.569583333301</v>
       </c>
@@ -16974,7 +17005,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>44533.605231481502</v>
       </c>
@@ -17097,7 +17128,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>44533.644687499997</v>
       </c>
@@ -17220,7 +17251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>44533.6639699074</v>
       </c>
@@ -17343,7 +17374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>44534.400462963</v>
       </c>
@@ -17466,7 +17497,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>44534.443124999998</v>
       </c>
@@ -17589,7 +17620,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>44534.450266203698</v>
       </c>
@@ -17712,7 +17743,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>44534.479016203702</v>
       </c>
@@ -17835,7 +17866,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>44534.539907407401</v>
       </c>
@@ -17958,7 +17989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>44534.596701388902</v>
       </c>
@@ -18081,7 +18112,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>44534.617881944403</v>
       </c>
@@ -18204,7 +18235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>44536.394675925898</v>
       </c>
@@ -18327,7 +18358,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>44536.4085416667</v>
       </c>
@@ -18450,7 +18481,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>44536.435104166703</v>
       </c>
@@ -18573,7 +18604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>44536.475509259297</v>
       </c>
@@ -18696,7 +18727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>44536.481076388904</v>
       </c>
@@ -18819,7 +18850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>44536.530312499999</v>
       </c>
@@ -18942,7 +18973,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>44536.530462962997</v>
       </c>
@@ -19065,7 +19096,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>44536.577118055597</v>
       </c>
@@ -19188,7 +19219,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>44536.6102314815</v>
       </c>
@@ -19311,7 +19342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>44536.697928240697</v>
       </c>
@@ -19434,7 +19465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>44537.397696759297</v>
       </c>
@@ -19557,7 +19588,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>44537.401377314804</v>
       </c>
@@ -19680,7 +19711,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="73" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>44537.440879629597</v>
       </c>
@@ -19803,7 +19834,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>44537.483495370398</v>
       </c>
@@ -19926,7 +19957,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>44537.534548611096</v>
       </c>
@@ -20049,7 +20080,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="76" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>44537.6180902778</v>
       </c>
@@ -20172,7 +20203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>44537.656435185199</v>
       </c>
@@ -20295,7 +20326,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>44537.667233796303</v>
       </c>
@@ -20418,7 +20449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>44537.698622685202</v>
       </c>
@@ -20541,7 +20572,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>44538.400277777801</v>
       </c>
@@ -20664,7 +20695,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>44538.406469907401</v>
       </c>
@@ -20787,7 +20818,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>44538.4353819444</v>
       </c>
@@ -20910,7 +20941,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>44538.496157407397</v>
       </c>
@@ -21033,7 +21064,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="84" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>44538.536446759303</v>
       </c>
@@ -21156,7 +21187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>44538.564131944397</v>
       </c>
@@ -21279,7 +21310,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>44538.628993055601</v>
       </c>
@@ -21402,7 +21433,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="87" spans="1:40" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:40" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>44538.658356481501</v>
       </c>
@@ -21525,7 +21556,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>44538.660694444399</v>
       </c>
@@ -21898,17 +21929,17 @@
       <selection activeCell="B43" sqref="A1:B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
@@ -21916,7 +21947,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -21924,7 +21955,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>7</v>
       </c>
@@ -21932,7 +21963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -21940,7 +21971,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -21948,7 +21979,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -21956,7 +21987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -21964,7 +21995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -21972,7 +22003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -21980,7 +22011,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -21988,7 +22019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
@@ -21996,7 +22027,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
@@ -22004,7 +22035,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>3</v>
       </c>
@@ -22012,7 +22043,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -22020,7 +22051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -22028,7 +22059,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
@@ -22036,7 +22067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -22044,7 +22075,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
@@ -22052,7 +22083,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -22060,7 +22091,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -22068,7 +22099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>3</v>
       </c>
@@ -22076,7 +22107,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7</v>
       </c>
@@ -22084,7 +22115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -22092,7 +22123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>5</v>
       </c>
@@ -22100,7 +22131,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -22108,7 +22139,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>5</v>
       </c>
@@ -22116,7 +22147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -22124,7 +22155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7</v>
       </c>
@@ -22132,7 +22163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>5</v>
       </c>
@@ -22140,7 +22171,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -22148,7 +22179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -22156,7 +22187,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>4</v>
       </c>
@@ -22164,7 +22195,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -22172,7 +22203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>3</v>
       </c>
@@ -22180,7 +22211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>3</v>
       </c>
@@ -22188,7 +22219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>3</v>
       </c>
@@ -22196,7 +22227,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>4</v>
       </c>
@@ -22204,7 +22235,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -22212,7 +22243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>4</v>
       </c>
@@ -22220,7 +22251,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>4</v>
       </c>
@@ -22228,7 +22259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>5</v>
       </c>
@@ -22236,7 +22267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -22257,17 +22288,17 @@
       <selection activeCell="B46" sqref="A1:B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>5</v>
       </c>
@@ -22275,7 +22306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -22283,7 +22314,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -22291,7 +22322,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -22299,7 +22330,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -22307,7 +22338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -22315,7 +22346,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -22323,7 +22354,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4</v>
       </c>
@@ -22331,7 +22362,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -22339,7 +22370,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -22347,7 +22378,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3</v>
       </c>
@@ -22355,7 +22386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -22363,7 +22394,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>5</v>
       </c>
@@ -22371,7 +22402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4</v>
       </c>
@@ -22379,7 +22410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
@@ -22387,7 +22418,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -22395,7 +22426,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
@@ -22403,7 +22434,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>3</v>
       </c>
@@ -22411,7 +22442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>3</v>
       </c>
@@ -22419,7 +22450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>4</v>
       </c>
@@ -22427,7 +22458,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>4</v>
       </c>
@@ -22435,7 +22466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -22443,7 +22474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>6</v>
       </c>
@@ -22451,7 +22482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>4</v>
       </c>
@@ -22459,7 +22490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -22467,7 +22498,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -22475,7 +22506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3</v>
       </c>
@@ -22483,7 +22514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -22491,7 +22522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4</v>
       </c>
@@ -22499,7 +22530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -22507,7 +22538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -22515,7 +22546,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>3</v>
       </c>
@@ -22523,7 +22554,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -22531,7 +22562,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -22539,7 +22570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -22547,7 +22578,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>4</v>
       </c>
@@ -22555,7 +22586,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6</v>
       </c>
@@ -22563,7 +22594,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>3</v>
       </c>
@@ -22571,7 +22602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>3</v>
       </c>
@@ -22579,7 +22610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -22587,7 +22618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>3</v>
       </c>
@@ -22595,7 +22626,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>3</v>
       </c>
@@ -22603,7 +22634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>5</v>
       </c>
@@ -22611,7 +22642,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1</v>
       </c>
@@ -22619,7 +22650,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>5</v>
       </c>
@@ -22640,9 +22671,9 @@
       <selection activeCell="E21" sqref="A1:F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -22662,7 +22693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>15</v>
       </c>
@@ -22682,7 +22713,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8</v>
       </c>
@@ -22702,7 +22733,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -22722,7 +22753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14</v>
       </c>
@@ -22742,7 +22773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -22762,7 +22793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>12</v>
       </c>
@@ -22782,7 +22813,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -22802,7 +22833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -22822,7 +22853,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>17</v>
       </c>
@@ -22842,7 +22873,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>12</v>
       </c>
@@ -22862,7 +22893,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -22882,7 +22913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5</v>
       </c>
@@ -22902,7 +22933,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -22922,7 +22953,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -22942,7 +22973,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>18</v>
       </c>
@@ -22962,7 +22993,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12</v>
       </c>
@@ -22982,7 +23013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -23002,7 +23033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -23022,7 +23053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
@@ -23042,7 +23073,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>13</v>
       </c>
@@ -23062,7 +23093,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
@@ -23082,7 +23113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>12</v>
       </c>
@@ -23102,7 +23133,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>16</v>
       </c>
@@ -23122,7 +23153,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>12</v>
       </c>
@@ -23142,7 +23173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>17</v>
       </c>
@@ -23162,7 +23193,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>13</v>
       </c>
@@ -23182,7 +23213,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>11</v>
       </c>
@@ -23202,7 +23233,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>18</v>
       </c>
@@ -23222,7 +23253,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -23242,7 +23273,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -23262,7 +23293,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>3</v>
       </c>
@@ -23282,7 +23313,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>15</v>
       </c>
@@ -23302,7 +23333,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>15</v>
       </c>
@@ -23322,7 +23353,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9</v>
       </c>
@@ -23342,7 +23373,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>14</v>
       </c>
@@ -23362,7 +23393,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>15</v>
       </c>
@@ -23382,7 +23413,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>15</v>
       </c>
@@ -23402,7 +23433,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>12</v>
       </c>
@@ -23422,7 +23453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>18</v>
       </c>
@@ -23442,7 +23473,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>13</v>
       </c>
@@ -23462,7 +23493,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>6</v>
       </c>
@@ -23482,7 +23513,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -23515,9 +23546,9 @@
       <selection activeCell="D20" sqref="A1:F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -23537,7 +23568,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>13</v>
       </c>
@@ -23557,7 +23588,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>12</v>
       </c>
@@ -23577,7 +23608,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8</v>
       </c>
@@ -23597,7 +23628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8</v>
       </c>
@@ -23617,7 +23648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>18</v>
       </c>
@@ -23637,7 +23668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>10</v>
       </c>
@@ -23657,7 +23688,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>12</v>
       </c>
@@ -23677,7 +23708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>15</v>
       </c>
@@ -23697,7 +23728,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -23717,7 +23748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -23737,7 +23768,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -23757,7 +23788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>14</v>
       </c>
@@ -23777,7 +23808,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -23797,7 +23828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>5</v>
       </c>
@@ -23817,7 +23848,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -23837,7 +23868,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -23857,7 +23888,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>13</v>
       </c>
@@ -23877,7 +23908,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -23897,7 +23928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>15</v>
       </c>
@@ -23917,7 +23948,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -23937,7 +23968,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>14</v>
       </c>
@@ -23957,7 +23988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>14</v>
       </c>
@@ -23977,7 +24008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>14</v>
       </c>
@@ -23997,7 +24028,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -24017,7 +24048,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>14</v>
       </c>
@@ -24037,7 +24068,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>19</v>
       </c>
@@ -24057,7 +24088,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>16</v>
       </c>
@@ -24077,7 +24108,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>15</v>
       </c>
@@ -24097,7 +24128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>12</v>
       </c>
@@ -24117,7 +24148,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>10</v>
       </c>
@@ -24137,7 +24168,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4</v>
       </c>
@@ -24157,7 +24188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -24177,7 +24208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>18</v>
       </c>
@@ -24197,7 +24228,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>15</v>
       </c>
@@ -24217,7 +24248,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11</v>
       </c>
@@ -24237,7 +24268,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>16</v>
       </c>
@@ -24257,7 +24288,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>7</v>
       </c>
@@ -24277,7 +24308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>10</v>
       </c>
@@ -24297,7 +24328,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>12</v>
       </c>
@@ -24317,7 +24348,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>5</v>
       </c>
@@ -24337,7 +24368,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>15</v>
       </c>
@@ -24357,7 +24388,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>16</v>
       </c>
@@ -24377,7 +24408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>16</v>
       </c>
@@ -24397,7 +24428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>8</v>
       </c>
@@ -24417,7 +24448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>4</v>
       </c>
@@ -24443,15 +24474,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B9EE4CF0A7BA564288E7D9A5DCD2046D" ma:contentTypeVersion="14" ma:contentTypeDescription="Opret et nyt dokument." ma:contentTypeScope="" ma:versionID="6f28af736a23b9f378c33a649ded4162">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6b4e5785-0607-4394-93a9-a60e4ad1cc61" xmlns:ns4="ef9cff76-29cd-40db-a37c-ecd9add28a83" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="370b35a3ac9ea8ec0a6b42bdb89ea4a7" ns3:_="" ns4:_="">
     <xsd:import namespace="6b4e5785-0607-4394-93a9-a60e4ad1cc61"/>
@@ -24680,21 +24702,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0344B36D-19B2-4291-9E00-F9DCE2483535}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9148981E-F5C3-4DEC-B879-01C130F2AC11}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24713,7 +24736,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3AE1981-EB7D-479B-A826-F05D1106B600}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -24728,4 +24751,12 @@
     <ds:schemaRef ds:uri="6b4e5785-0607-4394-93a9-a60e4ad1cc61"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0344B36D-19B2-4291-9E00-F9DCE2483535}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>